<commit_message>
Muestra bien los datos
</commit_message>
<xml_diff>
--- a/Back_end_python/db/poblacion.xlsx
+++ b/Back_end_python/db/poblacion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenin\Documents\GitHub\Python_AnalisisdeDatosCENSO\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenin\Documents\GitHub\Proyecto_python\Back_end_python\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B1E294-2336-40DD-82B4-3E300223AAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0CBFD6-2AB7-46B7-9EBA-F56BAA49ECE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D40FDDE0-FFB0-4579-BB60-701A6F5A9F65}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Censo de Población y Vivienda El Salvador 2024</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>La Unión</t>
-  </si>
-  <si>
-    <t>Nacional</t>
   </si>
   <si>
     <t>Fuente: Banco Central de Reserva de El Salvador</t>
@@ -316,7 +313,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -336,20 +333,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -679,29 +670,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9102632-BD08-419E-9BBA-5CE754B3048D}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="12" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" thickBot="1">
-      <c r="A1" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="A1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="42" customHeight="1" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -734,7 +724,7 @@
         <v>348880</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E16" si="0">D3/SUM($D$3:$D$16)</f>
+        <f>D3/SUM($D$3:$D$16)</f>
         <v>5.8903368793877212E-2</v>
       </c>
     </row>
@@ -752,7 +742,7 @@
         <v>552938</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E3:E16" si="0">D4/SUM($D$3:$D$16)</f>
         <v>9.3355626387723226E-2</v>
       </c>
     </row>
@@ -972,25 +962,6 @@
         <v>3.7882490750763012E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="7">
-        <v>2848533</v>
-      </c>
-      <c r="C17" s="7">
-        <v>3181443</v>
-      </c>
-      <c r="D17" s="7">
-        <f>C17+B17</f>
-        <v>6029976</v>
-      </c>
-      <c r="E17" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
@@ -1015,46 +986,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" ht="20.25" thickBot="1">
-      <c r="A2" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="A2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" ht="25.5" customHeight="1" thickTop="1">
-      <c r="A3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="11"/>
+      <c r="B4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="13"/>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2">
         <v>190284</v>
@@ -1068,7 +1039,7 @@
     </row>
     <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2">
         <v>230204</v>
@@ -1082,7 +1053,7 @@
     </row>
     <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2">
         <v>242611</v>
@@ -1096,7 +1067,7 @@
     </row>
     <row r="8" spans="1:4" ht="15.75">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2">
         <v>224736</v>
@@ -1110,7 +1081,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2">
         <v>250051</v>
@@ -1124,7 +1095,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2">
         <v>258535</v>
@@ -1138,7 +1109,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2">
         <v>231189</v>
@@ -1152,7 +1123,7 @@
     </row>
     <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2">
         <v>197824</v>
@@ -1166,7 +1137,7 @@
     </row>
     <row r="13" spans="1:4" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2">
         <v>183820</v>
@@ -1180,7 +1151,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2">
         <v>174197</v>
@@ -1194,7 +1165,7 @@
     </row>
     <row r="15" spans="1:4" ht="15.75">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2">
         <v>155246</v>
@@ -1208,7 +1179,7 @@
     </row>
     <row r="16" spans="1:4" ht="15.75">
       <c r="A16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="2">
         <v>128168</v>
@@ -1222,7 +1193,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2">
         <v>110386</v>
@@ -1236,7 +1207,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2">
         <v>86549</v>
@@ -1250,7 +1221,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2">
         <v>70715</v>
@@ -1264,7 +1235,7 @@
     </row>
     <row r="20" spans="1:4" ht="15.75">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2">
         <v>50342</v>
@@ -1278,7 +1249,7 @@
     </row>
     <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2">
         <v>33319</v>
@@ -1292,7 +1263,7 @@
     </row>
     <row r="22" spans="1:4" ht="15.75">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="2">
         <v>18979</v>
@@ -1306,7 +1277,7 @@
     </row>
     <row r="23" spans="1:4" ht="15.75">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2">
         <v>8273</v>
@@ -1320,7 +1291,7 @@
     </row>
     <row r="24" spans="1:4" ht="15.75">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2">
         <v>3105</v>
@@ -1347,12 +1318,12 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A26" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
+      <c r="A26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1367,6 +1338,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="27160ef2-b1a0-4e0b-a979-9938934b2ceb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="313f4996-b919-4f00-b21c-15f2583e5308" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009DCC8FD18B82734DA6D04F28797DC4A6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d6bdc30562d183d288a9000ae6c88d0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="27160ef2-b1a0-4e0b-a979-9938934b2ceb" xmlns:ns3="313f4996-b919-4f00-b21c-15f2583e5308" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb1f178905c4cbe79baa28c8245f5f7a" ns2:_="" ns3:_="">
     <xsd:import namespace="27160ef2-b1a0-4e0b-a979-9938934b2ceb"/>
@@ -1595,27 +1586,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5E9C4E8-A59C-4EC9-8806-F8CC90262200}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="27160ef2-b1a0-4e0b-a979-9938934b2ceb"/>
+    <ds:schemaRef ds:uri="313f4996-b919-4f00-b21c-15f2583e5308"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="27160ef2-b1a0-4e0b-a979-9938934b2ceb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="313f4996-b919-4f00-b21c-15f2583e5308" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8624A8-2CD9-429F-B7D5-684D5D2EBB1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34FBAE0C-E15C-4A27-A2B5-82CF1F9C3708}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1632,23 +1622,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8624A8-2CD9-429F-B7D5-684D5D2EBB1E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5E9C4E8-A59C-4EC9-8806-F8CC90262200}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="27160ef2-b1a0-4e0b-a979-9938934b2ceb"/>
-    <ds:schemaRef ds:uri="313f4996-b919-4f00-b21c-15f2583e5308"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>